<commit_message>
fixed determination of existing models; started implementing actor bulk
</commit_message>
<xml_diff>
--- a/repair/apps/asmfa/tests/data/T3.2_Activities_missing_relation.xlsx
+++ b/repair/apps/asmfa/tests/data/T3.2_Activities_missing_relation.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ggr Projekte\REPAiR-Web\repair\apps\asmfa\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F5C80A4-00E6-4312-AF12-A769872283E1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288D0DE5-3995-4823-A7E9-5EA1F42CD58B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21510" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21510" windowHeight="7935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T3.2_Activities_missing_relatio" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>NACE</t>
   </si>
@@ -31,154 +31,85 @@
     <t>AG</t>
   </si>
   <si>
-    <t>F-4110</t>
-  </si>
-  <si>
     <t>F-4110 Development of building projects</t>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
-    <t>F-4211</t>
-  </si>
-  <si>
     <t>F-4211 Construction of roads and motorways</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
-    <t>F-4120</t>
-  </si>
-  <si>
     <t>F-4120 Construction of residential and non-residential buildings</t>
   </si>
   <si>
     <t>Z</t>
   </si>
   <si>
-    <t>F-4221</t>
-  </si>
-  <si>
     <t>F-4221 Construction of utility projects for fluids</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>F-4399</t>
-  </si>
-  <si>
     <t>F-4399 Other specialised construction activities n.e.c.</t>
   </si>
   <si>
-    <t>F-4391</t>
-  </si>
-  <si>
     <t>F-4391 Roofing activities</t>
   </si>
   <si>
-    <t>F-4222</t>
-  </si>
-  <si>
     <t>F-4222 Construction of utility projects for electricity and telecommunications</t>
   </si>
   <si>
-    <t>F-4291</t>
-  </si>
-  <si>
     <t>F-4291 Construction of water projects</t>
   </si>
   <si>
-    <t>F-4299</t>
-  </si>
-  <si>
     <t>F-4299 Construction of other civil engineering projects n.e.c.</t>
   </si>
   <si>
-    <t>F-4212</t>
-  </si>
-  <si>
     <t>F-4212 Construction of railways and underground railwaysÊ</t>
   </si>
   <si>
-    <t>F-4333</t>
-  </si>
-  <si>
     <t>F-4333 Floor and wall covering</t>
   </si>
   <si>
-    <t>F-4329</t>
-  </si>
-  <si>
     <t>F-4329 Other construction installation</t>
   </si>
   <si>
-    <t>F-4332</t>
-  </si>
-  <si>
     <t>F-4332 Joinery installation</t>
   </si>
   <si>
-    <t>F-4213</t>
-  </si>
-  <si>
     <t>F-4213 Construction of bridges and tunnels</t>
   </si>
   <si>
-    <t>F-4339</t>
-  </si>
-  <si>
     <t>F-4339 Other building completion and finishing</t>
   </si>
   <si>
-    <t>F-4312</t>
-  </si>
-  <si>
     <t>F-4312 Site preparation</t>
   </si>
   <si>
-    <t>F-4311</t>
-  </si>
-  <si>
     <t>F-4311 Demolition</t>
   </si>
   <si>
-    <t>E-3821</t>
-  </si>
-  <si>
     <t>E-3821 Treatment and disposal of non-hazardous waste</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
-    <t>E-3811</t>
-  </si>
-  <si>
     <t>E-3811 Collection of non-hazardous waste</t>
   </si>
   <si>
-    <t>E-3832</t>
-  </si>
-  <si>
     <t>E-3832 Recovery of sorted materials</t>
   </si>
   <si>
-    <t>E-3900</t>
-  </si>
-  <si>
     <t>E-3900 Remediation activities and other waste management services</t>
   </si>
   <si>
-    <t>E-3822</t>
-  </si>
-  <si>
     <t>E-3822 Treatment and disposal of hazardous waste</t>
-  </si>
-  <si>
-    <t>E-3812</t>
   </si>
   <si>
     <t>E-3812 Collection of hazardous waste</t>
@@ -187,7 +118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1021,10 +952,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1040,256 +973,256 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>4110</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4211</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4120</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4221</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4399</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4391</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4222</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4291</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4299</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4212</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4333</v>
+      </c>
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4329</v>
+      </c>
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4332</v>
+      </c>
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4213</v>
+      </c>
+      <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4339</v>
+      </c>
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4312</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4311</v>
+      </c>
+      <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3821</v>
+      </c>
+      <c r="B19" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3811</v>
+      </c>
+      <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3832</v>
+      </c>
+      <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3900</v>
+      </c>
+      <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3822</v>
+      </c>
+      <c r="B23" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3812</v>
+      </c>
+      <c r="B24" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" t="s">
-        <v>53</v>
-      </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>